<commit_message>
update xlsx example, for dempo paper
</commit_message>
<xml_diff>
--- a/AutoGen/test_unit.xlsx
+++ b/AutoGen/test_unit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florianhofer/Documents/PhD-Research/projectControl/codeBase/IEC_61131-3_TestLib/AutoGen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845C8B92-7E88-3E4A-955B-1147E7B6C041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35891EF-7056-DA48-B9B5-CF299F486490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18940" windowHeight="13680" tabRatio="996" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18940" windowHeight="13680" tabRatio="996" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="s_battery" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1078,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Autogen: updated excel table and exp output to match SR test
</commit_message>
<xml_diff>
--- a/AutoGen/test_unit.xlsx
+++ b/AutoGen/test_unit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florianhofer/Documents/PhD-Research/projectControl/codeBase/IEC_61131-3_TestLib/AutoGen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD07982B-B69A-9F45-9DA8-A42B9C2AE346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508E3264-5DC5-834C-A8DB-266E93FF2970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9860" yWindow="500" windowWidth="18940" windowHeight="13680" tabRatio="996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9860" yWindow="4320" windowWidth="18940" windowHeight="13680" tabRatio="996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SERVER_ROOM" sheetId="4" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>BOOL</t>
   </si>
   <si>
-    <t xml:space="preserve">Room(Run := TRUE, Temp:= 20.1); (∗ start temp ∗) </t>
-  </si>
-  <si>
     <t>SERVER_ROOM</t>
   </si>
   <si>
@@ -126,19 +123,22 @@
     <t>2000, 25.1</t>
   </si>
   <si>
-    <t>3000, 23.0</t>
-  </si>
-  <si>
     <t>Tuple</t>
   </si>
   <si>
     <t>1000, 23.1</t>
   </si>
   <si>
-    <t xml:space="preserve">0, 22.1  </t>
-  </si>
-  <si>
     <t>BFRNG, 100</t>
+  </si>
+  <si>
+    <t>0, 22.1</t>
+  </si>
+  <si>
+    <t>3000, 22.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room(Run := TRUE, Temp:= 20.1); (* start temp *) </t>
   </si>
 </sst>
 </file>
@@ -622,7 +622,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -638,20 +638,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -735,7 +735,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -778,10 +778,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H8" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>12</v>
@@ -798,7 +798,7 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C9" s="9" t="b">
         <v>1</v>
@@ -809,7 +809,7 @@
       </c>
       <c r="F9" s="4"/>
       <c r="H9" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="8" t="s">
@@ -820,7 +820,7 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="C10" s="9" t="b">
         <v>0</v>
@@ -831,7 +831,7 @@
       </c>
       <c r="F10" s="4"/>
       <c r="H10" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="8" t="s">
@@ -847,7 +847,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C12" s="9" t="b">
         <v>0</v>
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H12" s="8" t="b">
         <v>1</v>
@@ -868,10 +868,10 @@
         <v>12</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
@@ -894,21 +894,21 @@
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C14" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="4"/>
       <c r="H14" s="8" t="b">
@@ -916,14 +916,14 @@
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="C15" s="9" t="b">
         <v>0</v>
@@ -938,7 +938,7 @@
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="K15" s="5"/>
     </row>

</xml_diff>